<commit_message>
run first trainings on simulid=30. something's wrong, as GPU% is stuck between 24% and 42%
</commit_message>
<xml_diff>
--- a/TestSet30.xlsx
+++ b/TestSet30.xlsx
@@ -118,6 +118,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -125,9 +128,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +433,7 @@
       <c r="C1" s="1">
         <v>30</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -441,12 +441,12 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -490,7 +490,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>9999</v>
+        <v>2728</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -507,22 +507,25 @@
       </c>
       <c r="F6" s="3" t="str">
         <f>$C$3&amp;" Infer "&amp;$C$1&amp;" "&amp;$C$2&amp;"Client.xml "&amp;$C$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A6</f>
-        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9999</v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2728</v>
       </c>
       <c r="G6" s="3" t="str">
         <f>$C$3&amp;" Infer "&amp;$C$1&amp;" "&amp;$C$2&amp;"Client.xml "&amp;$C$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A6</f>
-        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9999</v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2728</v>
       </c>
       <c r="H6" s="3" t="str">
         <f>$C$3&amp;" Infer "&amp;$C$1&amp;" "&amp;$C$2&amp;"Client.xml "&amp;$C$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A6</f>
-        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9999</v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2728</v>
       </c>
       <c r="I6" s="3" t="str">
         <f>$C$3&amp;" Infer "&amp;$C$1&amp;" "&amp;$C$2&amp;"Client.xml "&amp;$C$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A6</f>
-        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9999</v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2728</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>9652</v>
+      </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
@@ -538,19 +541,19 @@
       </c>
       <c r="F7" s="3" t="str">
         <f t="shared" ref="F7:I29" si="1">$C$3&amp;" Infer "&amp;$C$1&amp;" "&amp;$C$2&amp;"Client.xml "&amp;$C$2&amp;"inferDataSet"&amp;F$3&amp;".xml "&amp;$A7</f>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9652</v>
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9652</v>
       </c>
       <c r="H7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9652</v>
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9652</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1260,10 +1263,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3">

</xml_diff>

<commit_message>
more tests. data don't make sense anymore
</commit_message>
<xml_diff>
--- a/TestSet30.xlsx
+++ b/TestSet30.xlsx
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +421,7 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" style="4" customWidth="1"/>
+    <col min="5" max="5" width="104.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" style="3" customWidth="1"/>
     <col min="7" max="9" width="14.85546875" customWidth="1"/>
   </cols>
@@ -625,6 +625,9 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>7652</v>
+      </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
@@ -640,22 +643,25 @@
       </c>
       <c r="F10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 7652</v>
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 7652</v>
       </c>
       <c r="H10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 7652</v>
       </c>
       <c r="I10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 7652</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>8384</v>
+      </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
@@ -671,22 +677,25 @@
       </c>
       <c r="F11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8384</v>
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8384</v>
       </c>
       <c r="H11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8384</v>
       </c>
       <c r="I11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8384</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>6600</v>
+      </c>
       <c r="B12">
         <v>2</v>
       </c>
@@ -702,22 +711,25 @@
       </c>
       <c r="F12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 6600</v>
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 6600</v>
       </c>
       <c r="H12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 6600</v>
       </c>
       <c r="I12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 6600</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2220</v>
+      </c>
       <c r="B13" s="4">
         <v>2</v>
       </c>
@@ -733,22 +745,25 @@
       </c>
       <c r="F13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2220</v>
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2220</v>
       </c>
       <c r="H13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2220</v>
       </c>
       <c r="I13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2220</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>6612</v>
+      </c>
       <c r="B14" s="4">
         <v>2</v>
       </c>
@@ -764,22 +779,25 @@
       </c>
       <c r="F14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 6612</v>
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 6612</v>
       </c>
       <c r="H14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 6612</v>
       </c>
       <c r="I14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 6612</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>9492</v>
+      </c>
       <c r="B15" s="4">
         <v>2</v>
       </c>
@@ -795,22 +813,25 @@
       </c>
       <c r="F15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9492</v>
       </c>
       <c r="G15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9492</v>
       </c>
       <c r="H15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9492</v>
       </c>
       <c r="I15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9492</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>5756</v>
+      </c>
       <c r="B16" s="4">
         <v>2</v>
       </c>
@@ -826,19 +847,19 @@
       </c>
       <c r="F16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5756</v>
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5756</v>
       </c>
       <c r="H16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5756</v>
       </c>
       <c r="I16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v>zzzR Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5756</v>
       </c>
     </row>
     <row r="17" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
more tests. also rewritten MQL5 trade logic. error still too high
</commit_message>
<xml_diff>
--- a/TestSet30.xlsx
+++ b/TestSet30.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>SimulId</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>SimulationId:</t>
+  </si>
+  <si>
+    <t>MEM!</t>
   </si>
 </sst>
 </file>
@@ -444,15 +447,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19:E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="29" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +550,7 @@
         <v>inferDS4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2092</v>
       </c>
@@ -563,31 +564,31 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C6&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B6&amp;".xml"</f>
+        <f t="shared" ref="E6:E29" si="1">$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C6&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B6&amp;".xml"</f>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$A6</f>
+        <f t="shared" ref="F6:F29" si="2">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$A6</f>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 2092</v>
       </c>
       <c r="G6" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A6</f>
+        <f t="shared" ref="G6:J29" si="3">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A6</f>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2092</v>
       </c>
       <c r="H6" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A6</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2092</v>
       </c>
       <c r="I6" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A6</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2092</v>
       </c>
       <c r="J6" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A6</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2092</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>9084</v>
       </c>
@@ -601,31 +602,31 @@
         <v>2</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C7&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D7&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B7&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F7" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D7&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 9084</v>
       </c>
       <c r="G7" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9084</v>
       </c>
       <c r="H7" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9084</v>
       </c>
       <c r="I7" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9084</v>
       </c>
       <c r="J7" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A7</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9084</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>10020</v>
       </c>
@@ -639,31 +640,31 @@
         <v>3</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C8&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D8&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B8&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F8" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D8&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10020</v>
       </c>
       <c r="G8" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10020</v>
       </c>
       <c r="H8" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10020</v>
       </c>
       <c r="I8" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10020</v>
       </c>
       <c r="J8" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A8</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10020</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>9252</v>
       </c>
@@ -677,31 +678,31 @@
         <v>4</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C9&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D9&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B9&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F9" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D9&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 9252</v>
       </c>
       <c r="G9" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9252</v>
       </c>
       <c r="H9" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9252</v>
       </c>
       <c r="I9" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9252</v>
       </c>
       <c r="J9" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A9</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9252</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9036</v>
       </c>
@@ -715,31 +716,31 @@
         <v>5</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C10&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D10&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B10&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F10" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D10&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 9036</v>
       </c>
       <c r="G10" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9036</v>
       </c>
       <c r="H10" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9036</v>
       </c>
       <c r="I10" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9036</v>
       </c>
       <c r="J10" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A10</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9036</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>8356</v>
       </c>
@@ -753,472 +754,490 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C11&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D11&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B11&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F11" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D11&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="2"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 8356</v>
       </c>
       <c r="G11" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8356</v>
       </c>
       <c r="H11" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8356</v>
       </c>
       <c r="I11" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8356</v>
       </c>
       <c r="J11" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A11</f>
+        <f t="shared" si="3"/>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8356</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>5448</v>
+        <v>2035</v>
       </c>
       <c r="B12" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C12&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D12&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B12&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F12" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D12&amp;".xml "&amp;$A12</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 5448</v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 2035</v>
       </c>
       <c r="G12" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A12</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5448</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2035</v>
       </c>
       <c r="H12" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A12</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5448</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2035</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A12</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5448</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2035</v>
       </c>
       <c r="J12" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A12</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5448</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2035</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>5672</v>
+        <v>3608</v>
       </c>
       <c r="B13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
       </c>
       <c r="E13" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C13&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D13&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B13&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F13" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D13&amp;".xml "&amp;$A13</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 5672</v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 3608</v>
       </c>
       <c r="G13" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A13</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5672</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 3608</v>
       </c>
       <c r="H13" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A13</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5672</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 3608</v>
       </c>
       <c r="I13" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A13</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5672</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 3608</v>
       </c>
       <c r="J13" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A13</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5672</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 3608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>10196</v>
+        <v>7716</v>
       </c>
       <c r="B14" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="4">
         <v>3</v>
       </c>
       <c r="E14" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C14&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D14&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B14&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F14" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D14&amp;".xml "&amp;$A14</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10196</v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 7716</v>
       </c>
       <c r="G14" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A14</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10196</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 7716</v>
       </c>
       <c r="H14" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A14</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10196</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 7716</v>
       </c>
       <c r="I14" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A14</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10196</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 7716</v>
       </c>
       <c r="J14" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A14</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 7716</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>1104</v>
+        <v>5576</v>
       </c>
       <c r="B15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="4">
         <v>4</v>
       </c>
       <c r="E15" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C15&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D15&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B15&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F15" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D15&amp;".xml "&amp;$A15</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 1104</v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 5576</v>
       </c>
       <c r="G15" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A15</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 1104</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5576</v>
       </c>
       <c r="H15" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A15</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 1104</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5576</v>
       </c>
       <c r="I15" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A15</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 1104</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5576</v>
       </c>
       <c r="J15" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A15</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 1104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5576</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>9808</v>
+        <v>8384</v>
       </c>
       <c r="B16" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="4">
         <v>5</v>
       </c>
       <c r="E16" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C16&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D16&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B16&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F16" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D16&amp;".xml "&amp;$A16</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 9808</v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 8384</v>
       </c>
       <c r="G16" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A16</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9808</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8384</v>
       </c>
       <c r="H16" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A16</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9808</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8384</v>
       </c>
       <c r="I16" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A16</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9808</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8384</v>
       </c>
       <c r="J16" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A16</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9808</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>5908</v>
+        <v>9968</v>
       </c>
       <c r="B17" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="4">
         <v>6</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C17&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D17&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B17&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F17" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D17&amp;".xml "&amp;$A17</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 5908</v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 9968</v>
       </c>
       <c r="G17" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A17</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5908</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9968</v>
       </c>
       <c r="H17" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A17</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5908</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9968</v>
       </c>
       <c r="I17" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A17</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5908</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9968</v>
       </c>
       <c r="J17" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A17</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5908</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9968</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>2035</v>
+        <v>5448</v>
       </c>
       <c r="B18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="E18" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C18&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D18&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B18&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F18" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D18&amp;".xml "&amp;$A18</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 2035</v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 5448</v>
       </c>
       <c r="G18" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A18</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2035</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5448</v>
       </c>
       <c r="H18" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A18</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2035</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5448</v>
       </c>
       <c r="I18" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A18</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2035</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5448</v>
       </c>
       <c r="J18" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A18</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2035</v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5448</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>5672</v>
+      </c>
       <c r="B19" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
       </c>
       <c r="E19" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C19&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D19&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B19&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F19" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D19&amp;".xml "&amp;$A19</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 5672</v>
       </c>
       <c r="G19" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A19</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5672</v>
       </c>
       <c r="H19" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A19</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5672</v>
       </c>
       <c r="I19" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A19</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5672</v>
       </c>
       <c r="J19" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A19</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5672</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>10196</v>
+      </c>
       <c r="B20" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="4">
         <v>3</v>
       </c>
       <c r="E20" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C20&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D20&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B20&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F20" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D20&amp;".xml "&amp;$A20</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10196</v>
       </c>
       <c r="G20" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A20</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10196</v>
       </c>
       <c r="H20" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A20</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10196</v>
       </c>
       <c r="I20" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A20</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10196</v>
       </c>
       <c r="J20" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A20</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10196</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>1104</v>
+      </c>
       <c r="B21" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="4">
         <v>4</v>
       </c>
       <c r="E21" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C21&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D21&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B21&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F21" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D21&amp;".xml "&amp;$A21</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 1104</v>
       </c>
       <c r="G21" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A21</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 1104</v>
       </c>
       <c r="H21" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A21</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 1104</v>
       </c>
       <c r="I21" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A21</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 1104</v>
       </c>
       <c r="J21" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A21</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 1104</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>9808</v>
+      </c>
       <c r="B22" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="4">
         <v>5</v>
       </c>
       <c r="E22" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C22&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D22&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B22&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F22" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D22&amp;".xml "&amp;$A22</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 9808</v>
       </c>
       <c r="G22" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A22</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9808</v>
       </c>
       <c r="H22" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A22</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9808</v>
       </c>
       <c r="I22" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A22</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9808</v>
       </c>
       <c r="J22" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A22</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9808</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>5908</v>
+      </c>
       <c r="B23" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="4">
         <v>6</v>
       </c>
       <c r="E23" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C23&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D23&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B23&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
+        <f t="shared" si="1"/>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F23" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D23&amp;".xml "&amp;$A23</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 5908</v>
       </c>
       <c r="G23" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A23</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5908</v>
       </c>
       <c r="H23" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A23</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5908</v>
       </c>
       <c r="I23" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A23</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5908</v>
       </c>
       <c r="J23" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A23</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5908</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="B24" s="4">
         <v>2</v>
       </c>
@@ -1229,31 +1248,34 @@
         <v>1</v>
       </c>
       <c r="E24" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C24&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D24&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B24&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F24" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D24&amp;".xml "&amp;$A24</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml MEM!</v>
       </c>
       <c r="G24" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A24</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H24" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A24</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I24" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A24</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J24" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A24</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="B25" s="4">
         <v>2</v>
       </c>
@@ -1264,31 +1286,34 @@
         <v>2</v>
       </c>
       <c r="E25" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C25&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D25&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B25&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F25" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D25&amp;".xml "&amp;$A25</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml MEM!</v>
       </c>
       <c r="G25" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A25</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H25" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A25</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I25" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A25</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J25" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A25</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="B26" s="4">
         <v>2</v>
       </c>
@@ -1299,31 +1324,34 @@
         <v>3</v>
       </c>
       <c r="E26" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C26&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D26&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B26&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F26" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D26&amp;".xml "&amp;$A26</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml MEM!</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A26</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H26" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A26</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I26" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A26</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J26" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A26</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="B27" s="4">
         <v>2</v>
       </c>
@@ -1334,31 +1362,34 @@
         <v>4</v>
       </c>
       <c r="E27" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C27&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D27&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B27&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F27" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D27&amp;".xml "&amp;$A27</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml MEM!</v>
       </c>
       <c r="G27" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A27</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H27" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A27</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I27" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A27</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J27" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A27</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="B28" s="4">
         <v>2</v>
       </c>
@@ -1369,31 +1400,34 @@
         <v>5</v>
       </c>
       <c r="E28" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C28&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D28&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B28&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F28" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D28&amp;".xml "&amp;$A28</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml MEM!</v>
       </c>
       <c r="G28" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A28</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H28" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A28</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I28" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A28</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J28" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A28</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="B29" s="4">
         <v>2</v>
       </c>
@@ -1404,48 +1438,37 @@
         <v>6</v>
       </c>
       <c r="E29" s="4" t="str">
-        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C29&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D29&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B29&amp;".xml"</f>
+        <f t="shared" si="1"/>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F29" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D29&amp;".xml "&amp;$A29</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
+        <f t="shared" si="2"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml MEM!</v>
       </c>
       <c r="G29" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A29</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H29" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A29</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I29" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A29</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J29" s="3" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A29</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="4" t="str">
-        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D31&amp;".xml "</f>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet.xml </v>
+        <f t="shared" si="3"/>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A5:J29">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
+    <sortState ref="A6:J29">
+      <sortCondition ref="B6:B29"/>
+      <sortCondition ref="C6:C29"/>
+      <sortCondition ref="D6:D29"/>
+    </sortState>
   </autoFilter>
   <sortState ref="A6:J29">
     <sortCondition ref="C6:C29"/>

</xml_diff>

<commit_message>
fixed bug in vXMLconfigs.sql
</commit_message>
<xml_diff>
--- a/TestSet30.xlsx
+++ b/TestSet30.xlsx
@@ -447,13 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="29" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25:A29"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,929 +548,1349 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>2092</v>
-      </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
       <c r="C6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f t="shared" ref="E6:E29" si="1">$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C6&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B6&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C6&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B6&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f t="shared" ref="F6:F29" si="2">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$A6</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 2092</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$A6</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
       </c>
       <c r="G6" s="3" t="str">
-        <f t="shared" ref="G6:J29" si="3">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A6</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2092</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A6</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H6" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2092</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A6</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I6" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2092</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A6</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J6" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2092</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A6</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>9084</v>
-      </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
       <c r="C7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C7&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D7&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B7&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F7" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 9084</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D7&amp;".xml "&amp;$A7</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
       </c>
       <c r="G7" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9084</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A7</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H7" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9084</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A7</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I7" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9084</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A7</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J7" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9084</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A7</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>10020</v>
-      </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="C8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C8&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D8&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B8&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F8" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10020</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D8&amp;".xml "&amp;$A8</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
       </c>
       <c r="G8" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10020</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A8</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H8" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10020</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A8</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I8" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10020</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A8</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J8" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10020</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A8</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>9252</v>
-      </c>
       <c r="B9" s="4">
         <v>1</v>
       </c>
       <c r="C9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C9&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D9&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B9&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F9" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 9252</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D9&amp;".xml "&amp;$A9</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="G9" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9252</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A9</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H9" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9252</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A9</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I9" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9252</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A9</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J9" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9252</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A9</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9036</v>
-      </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
       <c r="C10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>5</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C10&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D10&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B10&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F10" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 9036</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D10&amp;".xml "&amp;$A10</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="G10" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9036</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A10</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H10" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9036</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A10</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I10" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9036</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A10</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J10" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9036</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A10</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>8356</v>
-      </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
       <c r="C11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>6</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C11&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D11&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B11&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F11" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 8356</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D11&amp;".xml "&amp;$A11</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="G11" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8356</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A11</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H11" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8356</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A11</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I11" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8356</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A11</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J11" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8356</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A11</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>2035</v>
+        <v>2092</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C12&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D12&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B12&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F12" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 2035</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D12&amp;".xml "&amp;$A12</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 2092</v>
       </c>
       <c r="G12" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2035</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A12</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2092</v>
       </c>
       <c r="H12" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2035</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A12</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2092</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2035</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A12</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2092</v>
       </c>
       <c r="J12" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2035</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A12</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2092</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>3608</v>
+        <v>9084</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
       </c>
       <c r="C13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
       </c>
       <c r="E13" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C13&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D13&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B13&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F13" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 3608</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D13&amp;".xml "&amp;$A13</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 9084</v>
       </c>
       <c r="G13" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 3608</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A13</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9084</v>
       </c>
       <c r="H13" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 3608</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A13</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9084</v>
       </c>
       <c r="I13" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 3608</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A13</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9084</v>
       </c>
       <c r="J13" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 3608</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A13</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9084</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>7716</v>
+        <v>10020</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="C14" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="4">
         <v>3</v>
       </c>
       <c r="E14" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C14&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D14&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B14&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F14" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 7716</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D14&amp;".xml "&amp;$A14</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10020</v>
       </c>
       <c r="G14" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 7716</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A14</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10020</v>
       </c>
       <c r="H14" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 7716</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A14</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10020</v>
       </c>
       <c r="I14" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 7716</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A14</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10020</v>
       </c>
       <c r="J14" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 7716</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A14</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10020</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>5576</v>
+        <v>9252</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="4">
         <v>4</v>
       </c>
       <c r="E15" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C15&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D15&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B15&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F15" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 5576</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D15&amp;".xml "&amp;$A15</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 9252</v>
       </c>
       <c r="G15" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5576</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A15</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9252</v>
       </c>
       <c r="H15" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5576</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A15</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9252</v>
       </c>
       <c r="I15" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5576</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A15</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9252</v>
       </c>
       <c r="J15" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5576</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A15</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9252</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>8384</v>
+        <v>9036</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
       <c r="C16" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="4">
         <v>5</v>
       </c>
       <c r="E16" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C16&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D16&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B16&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F16" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 8384</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D16&amp;".xml "&amp;$A16</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 9036</v>
       </c>
       <c r="G16" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8384</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A16</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9036</v>
       </c>
       <c r="H16" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8384</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A16</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9036</v>
       </c>
       <c r="I16" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8384</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A16</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9036</v>
       </c>
       <c r="J16" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8384</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A16</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9036</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>9968</v>
+        <v>8356</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
       </c>
       <c r="C17" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="4">
         <v>6</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C17&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D17&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B17&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F17" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 9968</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D17&amp;".xml "&amp;$A17</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 8356</v>
       </c>
       <c r="G17" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9968</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A17</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8356</v>
       </c>
       <c r="H17" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9968</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A17</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8356</v>
       </c>
       <c r="I17" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9968</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A17</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8356</v>
       </c>
       <c r="J17" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9968</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A17</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8356</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>5448</v>
+        <v>2035</v>
       </c>
       <c r="B18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="E18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C18&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D18&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B18&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F18" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 5448</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D18&amp;".xml "&amp;$A18</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 2035</v>
       </c>
       <c r="G18" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5448</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A18</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2035</v>
       </c>
       <c r="H18" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5448</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A18</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2035</v>
       </c>
       <c r="I18" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5448</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A18</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2035</v>
       </c>
       <c r="J18" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5448</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A18</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2035</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>5672</v>
+        <v>3608</v>
       </c>
       <c r="B19" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
       </c>
       <c r="E19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C19&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D19&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B19&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F19" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 5672</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D19&amp;".xml "&amp;$A19</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 3608</v>
       </c>
       <c r="G19" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5672</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A19</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 3608</v>
       </c>
       <c r="H19" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5672</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A19</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 3608</v>
       </c>
       <c r="I19" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5672</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A19</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 3608</v>
       </c>
       <c r="J19" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5672</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A19</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 3608</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>10196</v>
+        <v>7716</v>
       </c>
       <c r="B20" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="4">
         <v>3</v>
       </c>
       <c r="E20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C20&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D20&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B20&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F20" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10196</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D20&amp;".xml "&amp;$A20</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 7716</v>
       </c>
       <c r="G20" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10196</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A20</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 7716</v>
       </c>
       <c r="H20" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10196</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A20</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 7716</v>
       </c>
       <c r="I20" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10196</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A20</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 7716</v>
       </c>
       <c r="J20" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10196</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A20</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 7716</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>1104</v>
+        <v>5576</v>
       </c>
       <c r="B21" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="4">
         <v>4</v>
       </c>
       <c r="E21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C21&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D21&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B21&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F21" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 1104</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D21&amp;".xml "&amp;$A21</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 5576</v>
       </c>
       <c r="G21" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 1104</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A21</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5576</v>
       </c>
       <c r="H21" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 1104</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A21</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5576</v>
       </c>
       <c r="I21" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 1104</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A21</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5576</v>
       </c>
       <c r="J21" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 1104</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A21</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5576</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>9808</v>
+        <v>8384</v>
       </c>
       <c r="B22" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="4">
         <v>5</v>
       </c>
       <c r="E22" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C22&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D22&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B22&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F22" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 9808</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D22&amp;".xml "&amp;$A22</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 8384</v>
       </c>
       <c r="G22" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9808</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A22</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8384</v>
       </c>
       <c r="H22" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9808</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A22</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8384</v>
       </c>
       <c r="I22" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9808</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A22</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8384</v>
       </c>
       <c r="J22" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9808</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A22</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8384</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>5908</v>
+        <v>9968</v>
       </c>
       <c r="B23" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="4">
         <v>6</v>
       </c>
       <c r="E23" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C23&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D23&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B23&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F23" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 5908</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D23&amp;".xml "&amp;$A23</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 9968</v>
       </c>
       <c r="G23" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5908</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A23</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9968</v>
       </c>
       <c r="H23" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5908</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A23</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9968</v>
       </c>
       <c r="I23" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5908</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A23</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9968</v>
       </c>
       <c r="J23" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5908</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A23</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9968</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="B24" s="4">
         <v>2</v>
       </c>
       <c r="C24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
       </c>
       <c r="E24" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C24&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D24&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B24&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F24" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D24&amp;".xml "&amp;$A24</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
       </c>
       <c r="G24" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A24</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H24" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A24</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I24" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A24</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J24" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A24</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="B25" s="4">
         <v>2</v>
       </c>
       <c r="C25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25" s="4">
         <v>2</v>
       </c>
       <c r="E25" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C25&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D25&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B25&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F25" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D25&amp;".xml "&amp;$A25</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
       </c>
       <c r="G25" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A25</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H25" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A25</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I25" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A25</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J25" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A25</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="B26" s="4">
         <v>2</v>
       </c>
       <c r="C26" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4">
         <v>3</v>
       </c>
       <c r="E26" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C26&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D26&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B26&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F26" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D26&amp;".xml "&amp;$A26</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
       </c>
       <c r="G26" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A26</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H26" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A26</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I26" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A26</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J26" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A26</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="B27" s="4">
         <v>2</v>
       </c>
       <c r="C27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4">
         <v>4</v>
       </c>
       <c r="E27" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C27&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D27&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B27&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F27" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D27&amp;".xml "&amp;$A27</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="G27" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A27</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H27" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A27</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I27" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A27</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J27" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A27</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="B28" s="4">
         <v>2</v>
       </c>
       <c r="C28" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" s="4">
         <v>5</v>
       </c>
       <c r="E28" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C28&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D28&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B28&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F28" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D28&amp;".xml "&amp;$A28</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="G28" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A28</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H28" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A28</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I28" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A28</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J28" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A28</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="B29" s="4">
         <v>2</v>
       </c>
       <c r="C29" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29" s="4">
         <v>6</v>
       </c>
       <c r="E29" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C29&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D29&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B29&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F29" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D29&amp;".xml "&amp;$A29</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
+      </c>
+      <c r="G29" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A29</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+      </c>
+      <c r="H29" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A29</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+      </c>
+      <c r="I29" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A29</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+      </c>
+      <c r="J29" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A29</f>
+        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>5448</v>
+      </c>
+      <c r="B30" s="4">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1</v>
+      </c>
+      <c r="E30" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C30&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D30&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B30&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F30" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D30&amp;".xml "&amp;$A30</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 5448</v>
+      </c>
+      <c r="G30" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A30</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5448</v>
+      </c>
+      <c r="H30" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A30</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5448</v>
+      </c>
+      <c r="I30" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A30</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5448</v>
+      </c>
+      <c r="J30" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A30</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5448</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>5672</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4">
+        <v>2</v>
+      </c>
+      <c r="E31" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C31&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D31&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B31&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F31" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D31&amp;".xml "&amp;$A31</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 5672</v>
+      </c>
+      <c r="G31" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A31</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5672</v>
+      </c>
+      <c r="H31" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A31</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5672</v>
+      </c>
+      <c r="I31" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A31</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5672</v>
+      </c>
+      <c r="J31" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A31</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5672</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>10196</v>
+      </c>
+      <c r="B32" s="4">
+        <v>2</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4">
+        <v>3</v>
+      </c>
+      <c r="E32" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C32&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D32&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B32&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F32" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D32&amp;".xml "&amp;$A32</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10196</v>
+      </c>
+      <c r="G32" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A32</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10196</v>
+      </c>
+      <c r="H32" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A32</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10196</v>
+      </c>
+      <c r="I32" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A32</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10196</v>
+      </c>
+      <c r="J32" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A32</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>1104</v>
+      </c>
+      <c r="B33" s="4">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <v>4</v>
+      </c>
+      <c r="E33" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C33&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D33&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B33&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F33" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D33&amp;".xml "&amp;$A33</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 1104</v>
+      </c>
+      <c r="G33" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A33</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 1104</v>
+      </c>
+      <c r="H33" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A33</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 1104</v>
+      </c>
+      <c r="I33" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A33</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 1104</v>
+      </c>
+      <c r="J33" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A33</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 1104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>9808</v>
+      </c>
+      <c r="B34" s="4">
+        <v>2</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4">
+        <v>5</v>
+      </c>
+      <c r="E34" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C34&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D34&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B34&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F34" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D34&amp;".xml "&amp;$A34</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 9808</v>
+      </c>
+      <c r="G34" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A34</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9808</v>
+      </c>
+      <c r="H34" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A34</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9808</v>
+      </c>
+      <c r="I34" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A34</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9808</v>
+      </c>
+      <c r="J34" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A34</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9808</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>5908</v>
+      </c>
+      <c r="B35" s="4">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+      <c r="D35" s="4">
+        <v>6</v>
+      </c>
+      <c r="E35" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C35&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D35&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B35&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F35" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D35&amp;".xml "&amp;$A35</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 5908</v>
+      </c>
+      <c r="G35" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A35</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5908</v>
+      </c>
+      <c r="H35" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A35</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5908</v>
+      </c>
+      <c r="I35" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A35</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5908</v>
+      </c>
+      <c r="J35" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A35</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5908</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="4">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C36&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D36&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B36&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F36" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D36&amp;".xml "&amp;$A36</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml MEM!</v>
+      </c>
+      <c r="G36" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A36</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+      </c>
+      <c r="H36" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A36</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+      </c>
+      <c r="I36" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A36</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+      </c>
+      <c r="J36" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A36</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="4">
+        <v>2</v>
+      </c>
+      <c r="C37" s="4">
+        <v>2</v>
+      </c>
+      <c r="D37" s="4">
+        <v>2</v>
+      </c>
+      <c r="E37" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C37&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D37&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B37&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F37" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D37&amp;".xml "&amp;$A37</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml MEM!</v>
+      </c>
+      <c r="G37" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A37</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+      </c>
+      <c r="H37" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A37</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+      </c>
+      <c r="I37" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A37</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+      </c>
+      <c r="J37" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A37</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="4">
+        <v>2</v>
+      </c>
+      <c r="C38" s="4">
+        <v>2</v>
+      </c>
+      <c r="D38" s="4">
+        <v>3</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C38&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D38&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B38&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F38" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D38&amp;".xml "&amp;$A38</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml MEM!</v>
+      </c>
+      <c r="G38" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A38</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+      </c>
+      <c r="H38" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A38</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+      </c>
+      <c r="I38" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A38</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+      </c>
+      <c r="J38" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A38</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="4">
+        <v>2</v>
+      </c>
+      <c r="C39" s="4">
+        <v>2</v>
+      </c>
+      <c r="D39" s="4">
+        <v>4</v>
+      </c>
+      <c r="E39" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C39&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D39&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B39&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F39" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D39&amp;".xml "&amp;$A39</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml MEM!</v>
+      </c>
+      <c r="G39" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A39</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+      </c>
+      <c r="H39" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A39</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+      </c>
+      <c r="I39" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A39</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+      </c>
+      <c r="J39" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A39</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="4">
+        <v>2</v>
+      </c>
+      <c r="C40" s="4">
+        <v>2</v>
+      </c>
+      <c r="D40" s="4">
+        <v>5</v>
+      </c>
+      <c r="E40" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C40&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D40&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B40&amp;".xml"</f>
+        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
+      </c>
+      <c r="F40" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D40&amp;".xml "&amp;$A40</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml MEM!</v>
+      </c>
+      <c r="G40" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A40</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+      </c>
+      <c r="H40" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A40</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+      </c>
+      <c r="I40" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A40</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+      </c>
+      <c r="J40" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A40</f>
+        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4">
+        <v>2</v>
+      </c>
+      <c r="D41" s="4">
+        <v>6</v>
+      </c>
+      <c r="E41" s="4" t="str">
+        <f>$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C41&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D41&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B41&amp;".xml"</f>
         <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
       </c>
-      <c r="F29" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="F41" s="4" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D41&amp;".xml "&amp;$A41</f>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml MEM!</v>
       </c>
-      <c r="G29" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="G41" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A41</f>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
-      <c r="H29" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="H41" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;H$3&amp;".xml "&amp;$A41</f>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
-      <c r="I29" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="I41" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;I$3&amp;".xml "&amp;$A41</f>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
-      <c r="J29" s="3" t="str">
-        <f t="shared" si="3"/>
+      <c r="J41" s="3" t="str">
+        <f>$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;J$3&amp;".xml "&amp;$A41</f>
         <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A5:J29">
     <sortState ref="A6:J29">
+      <sortCondition ref="C6:C29"/>
       <sortCondition ref="B6:B29"/>
-      <sortCondition ref="C6:C29"/>
       <sortCondition ref="D6:D29"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A6:J29">
-    <sortCondition ref="C6:C29"/>
-    <sortCondition ref="B6:B29"/>
-    <sortCondition ref="D6:D29"/>
+  <sortState ref="A6:J41">
+    <sortCondition ref="B6:B41"/>
+    <sortCondition ref="C6:C41"/>
+    <sortCondition ref="D6:D41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
SCGD now uses MaxEpochs as maxK. more tests on lower MaxEpochs
</commit_message>
<xml_diff>
--- a/TestSet30.xlsx
+++ b/TestSet30.xlsx
@@ -447,13 +447,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomRight" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>7</v>
@@ -564,28 +564,28 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f t="shared" ref="E6:E59" si="1">$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C6&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B6&amp;".xml"</f>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
+        <f t="shared" ref="E6:E60" si="1">$D$3&amp;" Both "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"DataShape"&amp;$C6&amp;".xml "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$D$2&amp;"Engine"&amp;$B6&amp;".xml"</f>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f t="shared" ref="F6:F59" si="2">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$A6</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 10408</v>
+        <f t="shared" ref="F6:F60" si="2">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml"&amp;" "&amp;$D$2&amp;"trainDataSet"&amp;$D6&amp;".xml "&amp;$A6</f>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 10408</v>
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" ref="G6:J25" si="3">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A6</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10408</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10408</v>
       </c>
       <c r="H6" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10408</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10408</v>
       </c>
       <c r="I6" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10408</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10408</v>
       </c>
       <c r="J6" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10408</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10408</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -603,27 +603,27 @@
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F7" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 9428</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 9428</v>
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9428</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9428</v>
       </c>
       <c r="H7" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9428</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9428</v>
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9428</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9428</v>
       </c>
       <c r="J7" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9428</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9428</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -641,27 +641,27 @@
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F8" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 7756</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 7756</v>
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 7756</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 7756</v>
       </c>
       <c r="H8" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 7756</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 7756</v>
       </c>
       <c r="I8" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 7756</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 7756</v>
       </c>
       <c r="J8" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 7756</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 7756</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -679,27 +679,27 @@
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F9" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 232</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml 232</v>
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 232</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 232</v>
       </c>
       <c r="H9" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 232</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 232</v>
       </c>
       <c r="I9" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 232</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 232</v>
       </c>
       <c r="J9" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 232</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 232</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -717,27 +717,27 @@
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F10" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 10028</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml 10028</v>
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10028</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10028</v>
       </c>
       <c r="H10" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10028</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10028</v>
       </c>
       <c r="I10" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10028</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10028</v>
       </c>
       <c r="J10" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10028</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10028</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -755,27 +755,27 @@
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F11" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 10512</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml 10512</v>
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10512</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10512</v>
       </c>
       <c r="H11" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10512</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10512</v>
       </c>
       <c r="I11" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10512</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10512</v>
       </c>
       <c r="J11" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10512</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10512</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -793,27 +793,27 @@
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F12" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 2092</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 2092</v>
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2092</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 2092</v>
       </c>
       <c r="H12" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2092</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 2092</v>
       </c>
       <c r="I12" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2092</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 2092</v>
       </c>
       <c r="J12" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2092</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 2092</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -831,27 +831,27 @@
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F13" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 9084</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 9084</v>
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9084</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9084</v>
       </c>
       <c r="H13" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9084</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9084</v>
       </c>
       <c r="I13" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9084</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9084</v>
       </c>
       <c r="J13" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9084</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9084</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -869,27 +869,27 @@
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F14" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10020</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 10020</v>
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10020</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10020</v>
       </c>
       <c r="H14" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10020</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10020</v>
       </c>
       <c r="I14" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10020</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10020</v>
       </c>
       <c r="J14" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10020</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10020</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -907,27 +907,27 @@
       </c>
       <c r="E15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F15" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 9252</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml 9252</v>
       </c>
       <c r="G15" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9252</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9252</v>
       </c>
       <c r="H15" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9252</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9252</v>
       </c>
       <c r="I15" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9252</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9252</v>
       </c>
       <c r="J15" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9252</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9252</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -945,27 +945,27 @@
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F16" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 9036</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml 9036</v>
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9036</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9036</v>
       </c>
       <c r="H16" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9036</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9036</v>
       </c>
       <c r="I16" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9036</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9036</v>
       </c>
       <c r="J16" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9036</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9036</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -983,27 +983,27 @@
       </c>
       <c r="E17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F17" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 8356</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml 8356</v>
       </c>
       <c r="G17" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8356</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 8356</v>
       </c>
       <c r="H17" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8356</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 8356</v>
       </c>
       <c r="I17" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8356</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 8356</v>
       </c>
       <c r="J17" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8356</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 8356</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1021,27 +1021,27 @@
       </c>
       <c r="E18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F18" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 2035</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 2035</v>
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 2035</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 2035</v>
       </c>
       <c r="H18" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 2035</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 2035</v>
       </c>
       <c r="I18" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 2035</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 2035</v>
       </c>
       <c r="J18" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 2035</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 2035</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1059,27 +1059,27 @@
       </c>
       <c r="E19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F19" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 3608</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 3608</v>
       </c>
       <c r="G19" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 3608</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 3608</v>
       </c>
       <c r="H19" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 3608</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 3608</v>
       </c>
       <c r="I19" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 3608</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 3608</v>
       </c>
       <c r="J19" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 3608</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 3608</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1097,27 +1097,27 @@
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F20" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 7716</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 7716</v>
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 7716</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 7716</v>
       </c>
       <c r="H20" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 7716</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 7716</v>
       </c>
       <c r="I20" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 7716</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 7716</v>
       </c>
       <c r="J20" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 7716</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 7716</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1135,27 +1135,27 @@
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F21" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 5576</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml 5576</v>
       </c>
       <c r="G21" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5576</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 5576</v>
       </c>
       <c r="H21" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5576</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 5576</v>
       </c>
       <c r="I21" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5576</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 5576</v>
       </c>
       <c r="J21" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5576</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 5576</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1173,27 +1173,27 @@
       </c>
       <c r="E22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F22" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 8384</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml 8384</v>
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8384</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 8384</v>
       </c>
       <c r="H22" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8384</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 8384</v>
       </c>
       <c r="I22" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8384</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 8384</v>
       </c>
       <c r="J22" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8384</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 8384</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1211,27 +1211,27 @@
       </c>
       <c r="E23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine1.xml</v>
       </c>
       <c r="F23" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 9968</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml 9968</v>
       </c>
       <c r="G23" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9968</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9968</v>
       </c>
       <c r="H23" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9968</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9968</v>
       </c>
       <c r="I23" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9968</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9968</v>
       </c>
       <c r="J23" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9968</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9968</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1249,27 +1249,27 @@
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F24" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 9288</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 9288</v>
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9288</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9288</v>
       </c>
       <c r="H24" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9288</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9288</v>
       </c>
       <c r="I24" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9288</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9288</v>
       </c>
       <c r="J24" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9288</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9288</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1287,27 +1287,27 @@
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F25" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 7680</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 7680</v>
       </c>
       <c r="G25" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 7680</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 7680</v>
       </c>
       <c r="H25" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 7680</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 7680</v>
       </c>
       <c r="I25" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 7680</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 7680</v>
       </c>
       <c r="J25" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 7680</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 7680</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1325,27 +1325,27 @@
       </c>
       <c r="E26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F26" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10292</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 10292</v>
       </c>
       <c r="G26" s="3" t="str">
         <f t="shared" ref="G26:J42" si="4">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A26</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10292</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10292</v>
       </c>
       <c r="H26" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10292</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10292</v>
       </c>
       <c r="I26" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10292</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10292</v>
       </c>
       <c r="J26" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10292</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10292</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1363,27 +1363,27 @@
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F27" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 3651</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml 3651</v>
       </c>
       <c r="G27" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 3651</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 3651</v>
       </c>
       <c r="H27" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 3651</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 3651</v>
       </c>
       <c r="I27" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 3651</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 3651</v>
       </c>
       <c r="J27" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 3651</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 3651</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1401,27 +1401,27 @@
       </c>
       <c r="E28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F28" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 11004</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml 11004</v>
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 11004</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 11004</v>
       </c>
       <c r="H28" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 11004</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 11004</v>
       </c>
       <c r="I28" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 11004</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 11004</v>
       </c>
       <c r="J28" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 11004</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 11004</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1439,27 +1439,27 @@
       </c>
       <c r="E29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F29" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 8812</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml 8812</v>
       </c>
       <c r="G29" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 8812</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 8812</v>
       </c>
       <c r="H29" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 8812</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 8812</v>
       </c>
       <c r="I29" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 8812</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 8812</v>
       </c>
       <c r="J29" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 8812</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 8812</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1477,27 +1477,27 @@
       </c>
       <c r="E30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F30" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 5448</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 5448</v>
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5448</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 5448</v>
       </c>
       <c r="H30" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5448</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 5448</v>
       </c>
       <c r="I30" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5448</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 5448</v>
       </c>
       <c r="J30" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5448</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 5448</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1515,27 +1515,27 @@
       </c>
       <c r="E31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F31" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 5672</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 5672</v>
       </c>
       <c r="G31" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5672</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 5672</v>
       </c>
       <c r="H31" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5672</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 5672</v>
       </c>
       <c r="I31" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5672</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 5672</v>
       </c>
       <c r="J31" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5672</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 5672</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1553,27 +1553,27 @@
       </c>
       <c r="E32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F32" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 10196</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 10196</v>
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 10196</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 10196</v>
       </c>
       <c r="H32" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 10196</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 10196</v>
       </c>
       <c r="I32" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 10196</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 10196</v>
       </c>
       <c r="J32" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 10196</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 10196</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1591,27 +1591,27 @@
       </c>
       <c r="E33" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F33" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 1104</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml 1104</v>
       </c>
       <c r="G33" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 1104</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 1104</v>
       </c>
       <c r="H33" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 1104</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 1104</v>
       </c>
       <c r="I33" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 1104</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 1104</v>
       </c>
       <c r="J33" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 1104</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 1104</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1629,27 +1629,27 @@
       </c>
       <c r="E34" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F34" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml 9808</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml 9808</v>
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9808</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9808</v>
       </c>
       <c r="H34" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9808</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9808</v>
       </c>
       <c r="I34" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9808</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9808</v>
       </c>
       <c r="J34" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9808</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9808</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1667,27 +1667,27 @@
       </c>
       <c r="E35" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F35" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml 5908</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml 5908</v>
       </c>
       <c r="G35" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5908</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 5908</v>
       </c>
       <c r="H35" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5908</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 5908</v>
       </c>
       <c r="I35" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5908</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 5908</v>
       </c>
       <c r="J35" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5908</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 5908</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1705,27 +1705,27 @@
       </c>
       <c r="E36" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F36" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml MEM!</v>
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H36" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I36" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J36" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1743,27 +1743,27 @@
       </c>
       <c r="E37" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F37" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml MEM!</v>
       </c>
       <c r="G37" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H37" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I37" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J37" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1781,27 +1781,27 @@
       </c>
       <c r="E38" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F38" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml MEM!</v>
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H38" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I38" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J38" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1819,27 +1819,27 @@
       </c>
       <c r="E39" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F39" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml MEM!</v>
       </c>
       <c r="G39" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H39" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I39" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J39" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1857,27 +1857,27 @@
       </c>
       <c r="E40" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F40" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml MEM!</v>
       </c>
       <c r="G40" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H40" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I40" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J40" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1895,27 +1895,27 @@
       </c>
       <c r="E41" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine2.xml</v>
       </c>
       <c r="F41" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml MEM!</v>
       </c>
       <c r="G41" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml MEM!</v>
       </c>
       <c r="H41" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml MEM!</v>
       </c>
       <c r="I41" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml MEM!</v>
       </c>
       <c r="J41" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml MEM!</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1933,27 +1933,27 @@
       </c>
       <c r="E42" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet1.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet1.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F42" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml 4800</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml 4800</v>
       </c>
       <c r="G42" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 4800</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 4800</v>
       </c>
       <c r="H42" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 4800</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 4800</v>
       </c>
       <c r="I42" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 4800</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 4800</v>
       </c>
       <c r="J42" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 4800</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 4800</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1971,27 +1971,27 @@
       </c>
       <c r="E43" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet2.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet2.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F43" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml 5260</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml 5260</v>
       </c>
       <c r="G43" s="3" t="str">
         <f t="shared" ref="G43:J59" si="5">$D$3&amp;" Infer "&amp;$D$1&amp;" "&amp;$D$2&amp;"Client.xml "&amp;$D$2&amp;"inferDataSet"&amp;G$3&amp;".xml "&amp;$A43</f>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 5260</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 5260</v>
       </c>
       <c r="H43" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 5260</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 5260</v>
       </c>
       <c r="I43" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 5260</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 5260</v>
       </c>
       <c r="J43" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 5260</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 5260</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2009,27 +2009,27 @@
       </c>
       <c r="E44" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet3.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet3.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F44" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml 96</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml 96</v>
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 96</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 96</v>
       </c>
       <c r="H44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 96</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 96</v>
       </c>
       <c r="I44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 96</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 96</v>
       </c>
       <c r="J44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 96</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 96</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2047,27 +2047,27 @@
       </c>
       <c r="E45" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet4.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet4.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F45" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml 9184</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml 9184</v>
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml 9184</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml 9184</v>
       </c>
       <c r="H45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml 9184</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml 9184</v>
       </c>
       <c r="I45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml 9184</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml 9184</v>
       </c>
       <c r="J45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml 9184</v>
+        <v>zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml 9184</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2082,27 +2082,27 @@
       </c>
       <c r="E46" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet5.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet5.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F46" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="G46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2117,27 +2117,27 @@
       </c>
       <c r="E47" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet6.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape0.xml Config/30/trainDataSet6.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F47" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2152,27 +2152,27 @@
       </c>
       <c r="E48" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet1.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F48" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
@@ -2187,27 +2187,27 @@
       </c>
       <c r="E49" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet2.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F49" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -2222,27 +2222,27 @@
       </c>
       <c r="E50" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet3.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F50" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
@@ -2257,27 +2257,27 @@
       </c>
       <c r="E51" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet4.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F51" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -2292,27 +2292,27 @@
       </c>
       <c r="E52" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet5.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F52" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -2327,27 +2327,27 @@
       </c>
       <c r="E53" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet6.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F53" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -2362,27 +2362,27 @@
       </c>
       <c r="E54" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet1.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F54" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet1.xml </v>
       </c>
       <c r="G54" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H54" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I54" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J54" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -2397,27 +2397,27 @@
       </c>
       <c r="E55" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet2.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F55" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet2.xml </v>
       </c>
       <c r="G55" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H55" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I55" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J55" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
@@ -2432,27 +2432,27 @@
       </c>
       <c r="E56" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet3.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F56" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet3.xml </v>
       </c>
       <c r="G56" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H56" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I56" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J56" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -2467,27 +2467,27 @@
       </c>
       <c r="E57" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet4.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F57" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet4.xml </v>
       </c>
       <c r="G57" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H57" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I57" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J57" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -2502,27 +2502,27 @@
       </c>
       <c r="E58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet5.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F58" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet5.xml </v>
       </c>
       <c r="G58" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H58" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I58" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J58" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
@@ -2537,27 +2537,46 @@
       </c>
       <c r="E59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>zzz Both 30 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine3.xml</v>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape2.xml Config/30/trainDataSet6.xml Config/30/Engine3.xml</v>
       </c>
       <c r="F59" s="4" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet6.xml </v>
       </c>
       <c r="G59" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet1.xml </v>
       </c>
       <c r="H59" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet2.xml </v>
       </c>
       <c r="I59" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet3.xml </v>
       </c>
       <c r="J59" s="3" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">zzz Infer 30 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/inferDataSet4.xml </v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>7</v>
+      </c>
+      <c r="E60" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>zzz Both 31 Config/30/Client.xml Config/30/DataShape1.xml Config/30/trainDataSet7.xml Config/30/Engine4.xml</v>
+      </c>
+      <c r="F60" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">zzz Infer 31 Config/30/Client.xml Config/30/trainDataSet7.xml </v>
       </c>
     </row>
   </sheetData>

</xml_diff>